<commit_message>
1.  transmision_edocs_bosch - se trabajando en la condiciones del armado sql, se generó la información en base a sql
2.  transmision_edocs_bosch - se adaptó las funciones de generación de Excel con los componentes ( SpreadsheetLight,   ClosedXML)
3. se generó los archivos con los componentes
</commit_message>
<xml_diff>
--- a/01-CodigoFuente/main/consulta_datos/db_cone/db_cone/bin/Debug/net8.0/closedXML.xlsx
+++ b/01-CodigoFuente/main/consulta_datos/db_cone/db_cone/bin/Debug/net8.0/closedXML.xlsx
@@ -65,10 +65,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="3">
+  <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <x:numFmt numFmtId="165" formatCode="$#,##0.000; ($#,##0.000)"/>
   </x:numFmts>
   <x:fonts count="1">
     <x:font>
@@ -106,27 +104,13 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -134,18 +118,13 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:dxfs count="1">
-    <x:dxf>
-      <x:numFmt numFmtId="164" formatCode="$#,##0.000; ($#,##0.000)"/>
-    </x:dxf>
-  </x:dxfs>
 </x:styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K2" totalsRowShown="0">
   <x:tableColumns count="11">
-    <x:tableColumn id="1" name="ID_REP" dataDxfId="0"/>
+    <x:tableColumn id="1" name="ID_REP"/>
     <x:tableColumn id="2" name="ID_CRON"/>
     <x:tableColumn id="3" name="NAME"/>
     <x:tableColumn id="4" name="CONFIRMACION"/>
@@ -483,7 +462,7 @@
       <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="1" t="s">
+      <x:c r="J1" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="K1" s="0" t="s">
@@ -491,7 +470,7 @@
       </x:c>
     </x:row>
     <x:row r="2" spans="1:11">
-      <x:c r="A2" s="2">
+      <x:c r="A2" s="0">
         <x:v>207</x:v>
       </x:c>
       <x:c r="B2" s="0">

</xml_diff>